<commit_message>
Added some empirical tests and ploting results
</commit_message>
<xml_diff>
--- a/benchmark_heart_res.xlsx
+++ b/benchmark_heart_res.xlsx
@@ -435,22 +435,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>330.6852543714</v>
+        <v>328.6670608596</v>
       </c>
       <c r="C2">
-        <v>15.4857910012</v>
+        <v>13.8896666801</v>
       </c>
       <c r="D2">
-        <v>0.1993638408</v>
+        <v>0.2009297849</v>
       </c>
       <c r="E2">
-        <v>0.0126193037</v>
+        <v>0.0124132872</v>
       </c>
       <c r="F2">
-        <v>1.0238658568</v>
+        <v>1.0194684532</v>
       </c>
       <c r="G2">
-        <v>0.0330283956</v>
+        <v>0.0297859789</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -458,22 +458,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>388.1279087207</v>
+        <v>391.6973940503</v>
       </c>
       <c r="C3">
-        <v>48.2412848434</v>
+        <v>36.1625748871</v>
       </c>
       <c r="D3">
-        <v>0.1162906875</v>
+        <v>0.1343657739</v>
       </c>
       <c r="E3">
-        <v>0.0807356425</v>
+        <v>0.0516522078</v>
       </c>
       <c r="F3">
-        <v>1.0063560203</v>
+        <v>1.0123951504</v>
       </c>
       <c r="G3">
-        <v>0.0567077927</v>
+        <v>0.0508387423</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -481,22 +481,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>325.2416052599</v>
+        <v>323.396516429</v>
       </c>
       <c r="C4">
-        <v>6.3182686057</v>
+        <v>3.0138386068</v>
       </c>
       <c r="D4">
-        <v>0.206067336</v>
+        <v>0.20871241</v>
       </c>
       <c r="E4">
-        <v>0.0113011807</v>
+        <v>0.009442055600000001</v>
       </c>
       <c r="F4">
-        <v>1.0036133244</v>
+        <v>1.0020165163</v>
       </c>
       <c r="G4">
-        <v>0.0080741982</v>
+        <v>0.004504653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>